<commit_message>
Support for property tax calculation, including standardDeduction
</commit_message>
<xml_diff>
--- a/tests/Feature/config/property_realistic.xlsx
+++ b/tests/Feature/config/property_realistic.xlsx
@@ -708,6 +708,8 @@
     <col min="32" max="32" width="12.854" bestFit="true" customWidth="true" style="0"/>
     <col min="33" max="33" width="16.425" bestFit="true" customWidth="true" style="0"/>
     <col min="34" max="34" width="17.567" bestFit="true" customWidth="true" style="0"/>
+    <col min="35" max="35" width="10.569" bestFit="true" customWidth="true" style="0"/>
+    <col min="36" max="36" width="9.283" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:39">
@@ -3746,10 +3748,10 @@
       </c>
       <c r="AD38" s="2"/>
       <c r="AE38" s="1">
-        <v>-215521.4</v>
+        <v>-219721.4</v>
       </c>
       <c r="AF38" s="1">
-        <v>-215521.4</v>
+        <v>-219721.4</v>
       </c>
       <c r="AG38" s="2"/>
       <c r="AH38" s="1">
@@ -3833,10 +3835,10 @@
       </c>
       <c r="AD39" s="9"/>
       <c r="AE39" s="8">
-        <v>-225466.62</v>
+        <v>-229918.62</v>
       </c>
       <c r="AF39" s="8">
-        <v>-440988.02</v>
+        <v>-449640.02</v>
       </c>
       <c r="AG39" s="9"/>
       <c r="AH39" s="8">
@@ -3920,10 +3922,10 @@
       </c>
       <c r="AD40" s="12"/>
       <c r="AE40" s="11">
-        <v>-219452.5686</v>
+        <v>-224232.1686</v>
       </c>
       <c r="AF40" s="11">
-        <v>-660440.5886</v>
+        <v>-673872.1886</v>
       </c>
       <c r="AG40" s="12"/>
       <c r="AH40" s="11">
@@ -4007,10 +4009,10 @@
       </c>
       <c r="AD41" s="2"/>
       <c r="AE41" s="1">
-        <v>-213566.1056</v>
+        <v>-218689.6856</v>
       </c>
       <c r="AF41" s="1">
-        <v>-874006.6942</v>
+        <v>-892561.8742</v>
       </c>
       <c r="AG41" s="2"/>
       <c r="AH41" s="1">
@@ -4094,10 +4096,10 @@
       </c>
       <c r="AD42" s="2"/>
       <c r="AE42" s="1">
-        <v>-212668.2496</v>
+        <v>-218153.0086</v>
       </c>
       <c r="AF42" s="1">
-        <v>-1086674.9438</v>
+        <v>-1110714.8828</v>
       </c>
       <c r="AG42" s="2"/>
       <c r="AH42" s="1">
@@ -4181,10 +4183,10 @@
       </c>
       <c r="AD43" s="2"/>
       <c r="AE43" s="1">
-        <v>-216088.422</v>
+        <v>-221952.42</v>
       </c>
       <c r="AF43" s="1">
-        <v>-1302763.3658</v>
+        <v>-1332667.3028</v>
       </c>
       <c r="AG43" s="2"/>
       <c r="AH43" s="1">
@@ -4268,10 +4270,10 @@
       </c>
       <c r="AD44" s="2"/>
       <c r="AE44" s="1">
-        <v>-219631.504</v>
+        <v>-225893.7019</v>
       </c>
       <c r="AF44" s="1">
-        <v>-1522394.8698</v>
+        <v>-1558561.0047</v>
       </c>
       <c r="AG44" s="2"/>
       <c r="AH44" s="1">
@@ -4355,10 +4357,10 @@
       </c>
       <c r="AD45" s="2"/>
       <c r="AE45" s="1">
-        <v>-223302.0156</v>
+        <v>-229982.3235</v>
       </c>
       <c r="AF45" s="1">
-        <v>-1745696.8854</v>
+        <v>-1788543.3282</v>
       </c>
       <c r="AG45" s="2"/>
       <c r="AH45" s="1">
@@ -4442,10 +4444,10 @@
       </c>
       <c r="AD46" s="2"/>
       <c r="AE46" s="1">
-        <v>-227106.288</v>
+        <v>-234225.6114</v>
       </c>
       <c r="AF46" s="1">
-        <v>-1972803.1734</v>
+        <v>-2022768.9396</v>
       </c>
       <c r="AG46" s="2"/>
       <c r="AH46" s="1">
@@ -4529,10 +4531,10 @@
       </c>
       <c r="AD47" s="2"/>
       <c r="AE47" s="1">
-        <v>-231049.3012</v>
+        <v>-238629.5914</v>
       </c>
       <c r="AF47" s="1">
-        <v>-2203852.4746</v>
+        <v>-2261398.531</v>
       </c>
       <c r="AG47" s="2"/>
       <c r="AH47" s="1">
@@ -4616,10 +4618,10 @@
       </c>
       <c r="AD48" s="2"/>
       <c r="AE48" s="1">
-        <v>-235137.0708</v>
+        <v>-243201.3753</v>
       </c>
       <c r="AF48" s="1">
-        <v>-2438989.5454</v>
+        <v>-2504599.9063</v>
       </c>
       <c r="AG48" s="2"/>
       <c r="AH48" s="1">
@@ -4703,10 +4705,10 @@
       </c>
       <c r="AD49" s="2"/>
       <c r="AE49" s="1">
-        <v>-239375.0868</v>
+        <v>-247947.606</v>
       </c>
       <c r="AF49" s="1">
-        <v>-2678364.6322</v>
+        <v>-2752547.5123</v>
       </c>
       <c r="AG49" s="2"/>
       <c r="AH49" s="1">
@@ -4790,10 +4792,10 @@
       </c>
       <c r="AD50" s="2"/>
       <c r="AE50" s="1">
-        <v>-243770.7104</v>
+        <v>-252876.8564</v>
       </c>
       <c r="AF50" s="1">
-        <v>-2922135.3426</v>
+        <v>-3005424.3687</v>
       </c>
       <c r="AG50" s="2"/>
       <c r="AH50" s="1">
@@ -4877,10 +4879,10 @@
       </c>
       <c r="AD51" s="2"/>
       <c r="AE51" s="1">
-        <v>-248330.7772</v>
+        <v>-257997.2305</v>
       </c>
       <c r="AF51" s="1">
-        <v>-3170466.1198</v>
+        <v>-3263421.5992</v>
       </c>
       <c r="AG51" s="2"/>
       <c r="AH51" s="1">
@@ -4964,10 +4966,10 @@
       </c>
       <c r="AD52" s="2"/>
       <c r="AE52" s="1">
-        <v>-253061.6472</v>
+        <v>-263316.4239</v>
       </c>
       <c r="AF52" s="1">
-        <v>-3423527.767</v>
+        <v>-3526738.0231</v>
       </c>
       <c r="AG52" s="2"/>
       <c r="AH52" s="1">
@@ -5051,10 +5053,10 @@
       </c>
       <c r="AD53" s="14"/>
       <c r="AE53" s="13">
-        <v>-257971.5716</v>
+        <v>-268844.0864</v>
       </c>
       <c r="AF53" s="13">
-        <v>-3681499.3386</v>
+        <v>-3795582.1095</v>
       </c>
       <c r="AG53" s="14"/>
       <c r="AH53" s="13">
@@ -5138,10 +5140,10 @@
       </c>
       <c r="AD54" s="2"/>
       <c r="AE54" s="1">
-        <v>-263067.5604</v>
+        <v>-274588.7001</v>
       </c>
       <c r="AF54" s="1">
-        <v>-3944566.899</v>
+        <v>-4070170.8096</v>
       </c>
       <c r="AG54" s="2"/>
       <c r="AH54" s="1">
@@ -5225,10 +5227,10 @@
       </c>
       <c r="AD55" s="2"/>
       <c r="AE55" s="1">
-        <v>-268358.5648</v>
+        <v>-280560.7618</v>
       </c>
       <c r="AF55" s="1">
-        <v>-4212925.4638</v>
+        <v>-4350731.5714</v>
       </c>
       <c r="AG55" s="2"/>
       <c r="AH55" s="1">
@@ -5312,10 +5314,10 @@
       </c>
       <c r="AD56" s="2"/>
       <c r="AE56" s="1">
-        <v>-273852.3048</v>
+        <v>-286769.6127</v>
       </c>
       <c r="AF56" s="1">
-        <v>-4486777.7686</v>
+        <v>-4637501.1841</v>
       </c>
       <c r="AG56" s="2"/>
       <c r="AH56" s="1">
@@ -5399,10 +5401,10 @@
       </c>
       <c r="AD57" s="14"/>
       <c r="AE57" s="13">
-        <v>-279558.4716</v>
+        <v>-293226.645</v>
       </c>
       <c r="AF57" s="13">
-        <v>-4766336.2402</v>
+        <v>-4930727.8291</v>
       </c>
       <c r="AG57" s="14"/>
       <c r="AH57" s="13">
@@ -5486,10 +5488,10 @@
       </c>
       <c r="AD58" s="2"/>
       <c r="AE58" s="1">
-        <v>-172661.5852</v>
+        <v>-187118.1679</v>
       </c>
       <c r="AF58" s="1">
-        <v>-4938997.8254</v>
+        <v>-5117845.997</v>
       </c>
       <c r="AG58" s="2"/>
       <c r="AH58" s="1">
@@ -5573,10 +5575,10 @@
       </c>
       <c r="AD59" s="2"/>
       <c r="AE59" s="1">
-        <v>-178820.1668</v>
+        <v>-194104.5779</v>
       </c>
       <c r="AF59" s="1">
-        <v>-5117817.9922</v>
+        <v>-5311950.5749</v>
       </c>
       <c r="AG59" s="2"/>
       <c r="AH59" s="1">
@@ -5660,10 +5662,10 @@
       </c>
       <c r="AD60" s="2"/>
       <c r="AE60" s="1">
-        <v>-185220.412</v>
+        <v>-201374.0446</v>
       </c>
       <c r="AF60" s="1">
-        <v>-5303038.4042</v>
+        <v>-5513324.6195</v>
       </c>
       <c r="AG60" s="2"/>
       <c r="AH60" s="1">
@@ -5747,10 +5749,10 @@
       </c>
       <c r="AD61" s="2"/>
       <c r="AE61" s="1">
-        <v>-191872.1608</v>
+        <v>-208938.4744</v>
       </c>
       <c r="AF61" s="1">
-        <v>-5494910.565</v>
+        <v>-5722263.0939</v>
       </c>
       <c r="AG61" s="2"/>
       <c r="AH61" s="1">
@@ -5834,10 +5836,10 @@
       </c>
       <c r="AD62" s="2"/>
       <c r="AE62" s="1">
-        <v>-198787.3644</v>
+        <v>-216811.9941</v>
       </c>
       <c r="AF62" s="1">
-        <v>-5693697.9294</v>
+        <v>-5939075.088</v>
       </c>
       <c r="AG62" s="2"/>
       <c r="AH62" s="1">
@@ -5921,10 +5923,10 @@
       </c>
       <c r="AD63" s="2"/>
       <c r="AE63" s="1">
-        <v>-205977.6784</v>
+        <v>-225008.5399</v>
       </c>
       <c r="AF63" s="1">
-        <v>-5899675.6078</v>
+        <v>-6164083.6279</v>
       </c>
       <c r="AG63" s="2"/>
       <c r="AH63" s="1">
@@ -6008,10 +6010,10 @@
       </c>
       <c r="AD64" s="2"/>
       <c r="AE64" s="1">
-        <v>-213456.104</v>
+        <v>-233543.5091</v>
       </c>
       <c r="AF64" s="1">
-        <v>-6113131.7118</v>
+        <v>-6397627.137</v>
       </c>
       <c r="AG64" s="2"/>
       <c r="AH64" s="1">
@@ -6095,10 +6097,10 @@
       </c>
       <c r="AD65" s="2"/>
       <c r="AE65" s="1">
-        <v>-221234.6212</v>
+        <v>-242431.3975</v>
       </c>
       <c r="AF65" s="1">
-        <v>-6334366.333</v>
+        <v>-6640058.5345</v>
       </c>
       <c r="AG65" s="2"/>
       <c r="AH65" s="1">
@@ -6182,10 +6184,10 @@
       </c>
       <c r="AD66" s="2"/>
       <c r="AE66" s="1">
-        <v>-229327.3912</v>
+        <v>-251689.006</v>
       </c>
       <c r="AF66" s="1">
-        <v>-6563693.7242</v>
+        <v>-6891747.5405</v>
       </c>
       <c r="AG66" s="2"/>
       <c r="AH66" s="1">
@@ -6269,10 +6271,10 @@
       </c>
       <c r="AD67" s="2"/>
       <c r="AE67" s="1">
-        <v>-237748.4196</v>
+        <v>-261333.1143</v>
       </c>
       <c r="AF67" s="1">
-        <v>-6801442.1438</v>
+        <v>-7153080.6548</v>
       </c>
       <c r="AG67" s="2"/>
       <c r="AH67" s="1">
@@ -6356,10 +6358,10 @@
       </c>
       <c r="AD68" s="2"/>
       <c r="AE68" s="1">
-        <v>-246512.372</v>
+        <v>-271381.3007</v>
       </c>
       <c r="AF68" s="1">
-        <v>-7047954.5158</v>
+        <v>-7424461.9555</v>
       </c>
       <c r="AG68" s="2"/>
       <c r="AH68" s="1">
@@ -6443,10 +6445,10 @@
       </c>
       <c r="AD69" s="2"/>
       <c r="AE69" s="1">
-        <v>-255635.3996</v>
+        <v>-281852.774</v>
       </c>
       <c r="AF69" s="1">
-        <v>-7303589.9154</v>
+        <v>-7706314.7295</v>
       </c>
       <c r="AG69" s="2"/>
       <c r="AH69" s="1">
@@ -6530,10 +6532,10 @@
       </c>
       <c r="AD70" s="2"/>
       <c r="AE70" s="1">
-        <v>-265133.588</v>
+        <v>-292766.8307</v>
       </c>
       <c r="AF70" s="1">
-        <v>-7568723.5034</v>
+        <v>-7999081.5602</v>
       </c>
       <c r="AG70" s="2"/>
       <c r="AH70" s="1">
@@ -6617,10 +6619,10 @@
       </c>
       <c r="AD71" s="2"/>
       <c r="AE71" s="1">
-        <v>-275023.7828</v>
+        <v>-304143.6869</v>
       </c>
       <c r="AF71" s="1">
-        <v>-7843747.2862</v>
+        <v>-8303225.2471</v>
       </c>
       <c r="AG71" s="2"/>
       <c r="AH71" s="1">
@@ -6704,10 +6706,10 @@
       </c>
       <c r="AD72" s="16"/>
       <c r="AE72" s="5">
-        <v>-285324.4352</v>
+        <v>-316005.3344</v>
       </c>
       <c r="AF72" s="5">
-        <v>-8129071.7214</v>
+        <v>-8619230.5815</v>
       </c>
       <c r="AG72" s="16"/>
       <c r="AH72" s="5">
@@ -7098,6 +7100,8 @@
     <col min="32" max="32" width="12.854" bestFit="true" customWidth="true" style="0"/>
     <col min="33" max="33" width="16.425" bestFit="true" customWidth="true" style="0"/>
     <col min="34" max="34" width="17.567" bestFit="true" customWidth="true" style="0"/>
+    <col min="35" max="35" width="10.569" bestFit="true" customWidth="true" style="0"/>
+    <col min="36" max="36" width="9.283" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:39">
@@ -7306,9 +7310,7 @@
       <c r="G6" s="1">
         <v>0.0</v>
       </c>
-      <c r="H6" s="2">
-        <v>0.22</v>
-      </c>
+      <c r="H6" s="2"/>
       <c r="I6" s="1"/>
       <c r="J6" s="2"/>
       <c r="K6" s="1"/>
@@ -7337,7 +7339,9 @@
         <v>0</v>
       </c>
       <c r="X6" s="2"/>
-      <c r="Y6" s="1"/>
+      <c r="Y6" s="1">
+        <v>0</v>
+      </c>
       <c r="Z6" s="2"/>
       <c r="AA6" s="1">
         <v>0.0</v>
@@ -7389,9 +7393,7 @@
       <c r="G7" s="1">
         <v>0.0</v>
       </c>
-      <c r="H7" s="2">
-        <v>0.22</v>
-      </c>
+      <c r="H7" s="2"/>
       <c r="I7" s="1"/>
       <c r="J7" s="2"/>
       <c r="K7" s="1"/>
@@ -7420,7 +7422,9 @@
         <v>0</v>
       </c>
       <c r="X7" s="2"/>
-      <c r="Y7" s="1"/>
+      <c r="Y7" s="1">
+        <v>0</v>
+      </c>
       <c r="Z7" s="2"/>
       <c r="AA7" s="1">
         <v>0.0</v>
@@ -7472,9 +7476,7 @@
       <c r="G8" s="1">
         <v>0.0</v>
       </c>
-      <c r="H8" s="2">
-        <v>0.22</v>
-      </c>
+      <c r="H8" s="2"/>
       <c r="I8" s="1"/>
       <c r="J8" s="2"/>
       <c r="K8" s="1"/>
@@ -7503,7 +7505,9 @@
         <v>0</v>
       </c>
       <c r="X8" s="2"/>
-      <c r="Y8" s="1"/>
+      <c r="Y8" s="1">
+        <v>0</v>
+      </c>
       <c r="Z8" s="2"/>
       <c r="AA8" s="1">
         <v>0.0</v>
@@ -7555,9 +7559,7 @@
       <c r="G9" s="1">
         <v>0.0</v>
       </c>
-      <c r="H9" s="2">
-        <v>0.22</v>
-      </c>
+      <c r="H9" s="2"/>
       <c r="I9" s="1"/>
       <c r="J9" s="2"/>
       <c r="K9" s="1"/>
@@ -7586,7 +7588,9 @@
         <v>0</v>
       </c>
       <c r="X9" s="2"/>
-      <c r="Y9" s="1"/>
+      <c r="Y9" s="1">
+        <v>0</v>
+      </c>
       <c r="Z9" s="2"/>
       <c r="AA9" s="1">
         <v>0.0</v>
@@ -7638,9 +7642,7 @@
       <c r="G10" s="1">
         <v>0.0</v>
       </c>
-      <c r="H10" s="2">
-        <v>0.22</v>
-      </c>
+      <c r="H10" s="2"/>
       <c r="I10" s="1"/>
       <c r="J10" s="2"/>
       <c r="K10" s="1"/>
@@ -7669,7 +7671,9 @@
         <v>0</v>
       </c>
       <c r="X10" s="2"/>
-      <c r="Y10" s="1"/>
+      <c r="Y10" s="1">
+        <v>0</v>
+      </c>
       <c r="Z10" s="2"/>
       <c r="AA10" s="1">
         <v>0.0</v>
@@ -7721,9 +7725,7 @@
       <c r="G11" s="1">
         <v>0.0</v>
       </c>
-      <c r="H11" s="2">
-        <v>0.22</v>
-      </c>
+      <c r="H11" s="2"/>
       <c r="I11" s="1"/>
       <c r="J11" s="2"/>
       <c r="K11" s="1"/>
@@ -7752,7 +7754,9 @@
         <v>0</v>
       </c>
       <c r="X11" s="2"/>
-      <c r="Y11" s="1"/>
+      <c r="Y11" s="1">
+        <v>0</v>
+      </c>
       <c r="Z11" s="2"/>
       <c r="AA11" s="1">
         <v>0.0</v>
@@ -7804,9 +7808,7 @@
       <c r="G12" s="1">
         <v>0.0</v>
       </c>
-      <c r="H12" s="2">
-        <v>0.22</v>
-      </c>
+      <c r="H12" s="2"/>
       <c r="I12" s="1"/>
       <c r="J12" s="2"/>
       <c r="K12" s="1"/>
@@ -7835,7 +7837,9 @@
         <v>0</v>
       </c>
       <c r="X12" s="2"/>
-      <c r="Y12" s="1"/>
+      <c r="Y12" s="1">
+        <v>0</v>
+      </c>
       <c r="Z12" s="2"/>
       <c r="AA12" s="1">
         <v>0.0</v>
@@ -7887,9 +7891,7 @@
       <c r="G13" s="1">
         <v>0.0</v>
       </c>
-      <c r="H13" s="2">
-        <v>0.22</v>
-      </c>
+      <c r="H13" s="2"/>
       <c r="I13" s="1"/>
       <c r="J13" s="2"/>
       <c r="K13" s="1"/>
@@ -7918,7 +7920,9 @@
         <v>0</v>
       </c>
       <c r="X13" s="2"/>
-      <c r="Y13" s="1"/>
+      <c r="Y13" s="1">
+        <v>0</v>
+      </c>
       <c r="Z13" s="2"/>
       <c r="AA13" s="1">
         <v>0.0</v>
@@ -7970,9 +7974,7 @@
       <c r="G14" s="1">
         <v>0.0</v>
       </c>
-      <c r="H14" s="2">
-        <v>0.22</v>
-      </c>
+      <c r="H14" s="2"/>
       <c r="I14" s="1"/>
       <c r="J14" s="2"/>
       <c r="K14" s="1"/>
@@ -8001,7 +8003,9 @@
         <v>0</v>
       </c>
       <c r="X14" s="2"/>
-      <c r="Y14" s="1"/>
+      <c r="Y14" s="1">
+        <v>0</v>
+      </c>
       <c r="Z14" s="2"/>
       <c r="AA14" s="1">
         <v>0.0</v>
@@ -8053,9 +8057,7 @@
       <c r="G15" s="1">
         <v>0.0</v>
       </c>
-      <c r="H15" s="2">
-        <v>0.22</v>
-      </c>
+      <c r="H15" s="2"/>
       <c r="I15" s="1"/>
       <c r="J15" s="2"/>
       <c r="K15" s="1"/>
@@ -8084,7 +8086,9 @@
         <v>0</v>
       </c>
       <c r="X15" s="2"/>
-      <c r="Y15" s="1"/>
+      <c r="Y15" s="1">
+        <v>0</v>
+      </c>
       <c r="Z15" s="2"/>
       <c r="AA15" s="1">
         <v>0.0</v>
@@ -8136,9 +8140,7 @@
       <c r="G16" s="1">
         <v>0.0</v>
       </c>
-      <c r="H16" s="2">
-        <v>0.22</v>
-      </c>
+      <c r="H16" s="2"/>
       <c r="I16" s="1"/>
       <c r="J16" s="2"/>
       <c r="K16" s="1"/>
@@ -8167,7 +8169,9 @@
         <v>0</v>
       </c>
       <c r="X16" s="2"/>
-      <c r="Y16" s="1"/>
+      <c r="Y16" s="1">
+        <v>0</v>
+      </c>
       <c r="Z16" s="2"/>
       <c r="AA16" s="1">
         <v>0.0</v>
@@ -8219,9 +8223,7 @@
       <c r="G17" s="1">
         <v>0.0</v>
       </c>
-      <c r="H17" s="2">
-        <v>0.22</v>
-      </c>
+      <c r="H17" s="2"/>
       <c r="I17" s="1"/>
       <c r="J17" s="2"/>
       <c r="K17" s="1"/>
@@ -8250,7 +8252,9 @@
         <v>0</v>
       </c>
       <c r="X17" s="2"/>
-      <c r="Y17" s="1"/>
+      <c r="Y17" s="1">
+        <v>0</v>
+      </c>
       <c r="Z17" s="2"/>
       <c r="AA17" s="1">
         <v>0.0</v>
@@ -8302,9 +8306,7 @@
       <c r="G18" s="1">
         <v>0.0</v>
       </c>
-      <c r="H18" s="2">
-        <v>0.22</v>
-      </c>
+      <c r="H18" s="2"/>
       <c r="I18" s="1"/>
       <c r="J18" s="2"/>
       <c r="K18" s="1"/>
@@ -8333,7 +8335,9 @@
         <v>0</v>
       </c>
       <c r="X18" s="2"/>
-      <c r="Y18" s="1"/>
+      <c r="Y18" s="1">
+        <v>0</v>
+      </c>
       <c r="Z18" s="2"/>
       <c r="AA18" s="1">
         <v>0.0</v>
@@ -8385,9 +8389,7 @@
       <c r="G19" s="1">
         <v>0.0</v>
       </c>
-      <c r="H19" s="2">
-        <v>0.22</v>
-      </c>
+      <c r="H19" s="2"/>
       <c r="I19" s="1"/>
       <c r="J19" s="2"/>
       <c r="K19" s="1"/>
@@ -8416,7 +8418,9 @@
         <v>0</v>
       </c>
       <c r="X19" s="2"/>
-      <c r="Y19" s="1"/>
+      <c r="Y19" s="1">
+        <v>0</v>
+      </c>
       <c r="Z19" s="2"/>
       <c r="AA19" s="1">
         <v>0.0</v>
@@ -8468,9 +8472,7 @@
       <c r="G20" s="1">
         <v>0.0</v>
       </c>
-      <c r="H20" s="2">
-        <v>0.22</v>
-      </c>
+      <c r="H20" s="2"/>
       <c r="I20" s="1"/>
       <c r="J20" s="2"/>
       <c r="K20" s="1"/>
@@ -8499,7 +8501,9 @@
         <v>0</v>
       </c>
       <c r="X20" s="2"/>
-      <c r="Y20" s="1"/>
+      <c r="Y20" s="1">
+        <v>0</v>
+      </c>
       <c r="Z20" s="2"/>
       <c r="AA20" s="1">
         <v>0.0</v>
@@ -8551,9 +8555,7 @@
       <c r="G21" s="1">
         <v>0.0</v>
       </c>
-      <c r="H21" s="2">
-        <v>0.22</v>
-      </c>
+      <c r="H21" s="2"/>
       <c r="I21" s="1"/>
       <c r="J21" s="2"/>
       <c r="K21" s="1"/>
@@ -8582,7 +8584,9 @@
         <v>0</v>
       </c>
       <c r="X21" s="2"/>
-      <c r="Y21" s="1"/>
+      <c r="Y21" s="1">
+        <v>0</v>
+      </c>
       <c r="Z21" s="2"/>
       <c r="AA21" s="1">
         <v>0.0</v>
@@ -8634,9 +8638,7 @@
       <c r="G22" s="1">
         <v>0.0</v>
       </c>
-      <c r="H22" s="2">
-        <v>0.22</v>
-      </c>
+      <c r="H22" s="2"/>
       <c r="I22" s="1"/>
       <c r="J22" s="2"/>
       <c r="K22" s="1"/>
@@ -8665,7 +8667,9 @@
         <v>0</v>
       </c>
       <c r="X22" s="2"/>
-      <c r="Y22" s="1"/>
+      <c r="Y22" s="1">
+        <v>0</v>
+      </c>
       <c r="Z22" s="2"/>
       <c r="AA22" s="1">
         <v>0.0</v>
@@ -8717,9 +8721,7 @@
       <c r="G23" s="1">
         <v>0.0</v>
       </c>
-      <c r="H23" s="2">
-        <v>0.22</v>
-      </c>
+      <c r="H23" s="2"/>
       <c r="I23" s="1"/>
       <c r="J23" s="2"/>
       <c r="K23" s="1"/>
@@ -8748,7 +8750,9 @@
         <v>0</v>
       </c>
       <c r="X23" s="2"/>
-      <c r="Y23" s="1"/>
+      <c r="Y23" s="1">
+        <v>0</v>
+      </c>
       <c r="Z23" s="2"/>
       <c r="AA23" s="1">
         <v>0.0</v>
@@ -8800,9 +8804,7 @@
       <c r="G24" s="1">
         <v>0.0</v>
       </c>
-      <c r="H24" s="2">
-        <v>0.22</v>
-      </c>
+      <c r="H24" s="2"/>
       <c r="I24" s="1"/>
       <c r="J24" s="2"/>
       <c r="K24" s="1"/>
@@ -8831,7 +8833,9 @@
         <v>0</v>
       </c>
       <c r="X24" s="2"/>
-      <c r="Y24" s="1"/>
+      <c r="Y24" s="1">
+        <v>0</v>
+      </c>
       <c r="Z24" s="2"/>
       <c r="AA24" s="1">
         <v>0.0</v>
@@ -8883,9 +8887,7 @@
       <c r="G25" s="1">
         <v>0.0</v>
       </c>
-      <c r="H25" s="2">
-        <v>0.22</v>
-      </c>
+      <c r="H25" s="2"/>
       <c r="I25" s="1"/>
       <c r="J25" s="2"/>
       <c r="K25" s="1"/>
@@ -8914,7 +8916,9 @@
         <v>0</v>
       </c>
       <c r="X25" s="2"/>
-      <c r="Y25" s="1"/>
+      <c r="Y25" s="1">
+        <v>0</v>
+      </c>
       <c r="Z25" s="2"/>
       <c r="AA25" s="1">
         <v>0.0</v>
@@ -8966,9 +8970,7 @@
       <c r="G26" s="1">
         <v>0.0</v>
       </c>
-      <c r="H26" s="2">
-        <v>0.22</v>
-      </c>
+      <c r="H26" s="2"/>
       <c r="I26" s="1"/>
       <c r="J26" s="2"/>
       <c r="K26" s="1"/>
@@ -8997,7 +8999,9 @@
         <v>0</v>
       </c>
       <c r="X26" s="2"/>
-      <c r="Y26" s="1"/>
+      <c r="Y26" s="1">
+        <v>0</v>
+      </c>
       <c r="Z26" s="2"/>
       <c r="AA26" s="1">
         <v>0.0</v>
@@ -9049,9 +9053,7 @@
       <c r="G27" s="1">
         <v>0.0</v>
       </c>
-      <c r="H27" s="2">
-        <v>0.22</v>
-      </c>
+      <c r="H27" s="2"/>
       <c r="I27" s="1"/>
       <c r="J27" s="2"/>
       <c r="K27" s="1"/>
@@ -9080,7 +9082,9 @@
         <v>0</v>
       </c>
       <c r="X27" s="2"/>
-      <c r="Y27" s="1"/>
+      <c r="Y27" s="1">
+        <v>0</v>
+      </c>
       <c r="Z27" s="2"/>
       <c r="AA27" s="1">
         <v>0.0</v>
@@ -9132,9 +9136,7 @@
       <c r="G28" s="1">
         <v>0.0</v>
       </c>
-      <c r="H28" s="2">
-        <v>0.22</v>
-      </c>
+      <c r="H28" s="2"/>
       <c r="I28" s="1"/>
       <c r="J28" s="2"/>
       <c r="K28" s="1"/>
@@ -9163,7 +9165,9 @@
         <v>0</v>
       </c>
       <c r="X28" s="2"/>
-      <c r="Y28" s="1"/>
+      <c r="Y28" s="1">
+        <v>0</v>
+      </c>
       <c r="Z28" s="2"/>
       <c r="AA28" s="1">
         <v>0.0</v>
@@ -9215,9 +9219,7 @@
       <c r="G29" s="1">
         <v>0.0</v>
       </c>
-      <c r="H29" s="2">
-        <v>0.22</v>
-      </c>
+      <c r="H29" s="2"/>
       <c r="I29" s="1"/>
       <c r="J29" s="2"/>
       <c r="K29" s="1"/>
@@ -9246,7 +9248,9 @@
         <v>0</v>
       </c>
       <c r="X29" s="2"/>
-      <c r="Y29" s="1"/>
+      <c r="Y29" s="1">
+        <v>0</v>
+      </c>
       <c r="Z29" s="2"/>
       <c r="AA29" s="1">
         <v>0.0</v>
@@ -9298,9 +9302,7 @@
       <c r="G30" s="1">
         <v>0.0</v>
       </c>
-      <c r="H30" s="2">
-        <v>0.22</v>
-      </c>
+      <c r="H30" s="2"/>
       <c r="I30" s="1"/>
       <c r="J30" s="2"/>
       <c r="K30" s="1"/>
@@ -9329,7 +9331,9 @@
         <v>0</v>
       </c>
       <c r="X30" s="2"/>
-      <c r="Y30" s="1"/>
+      <c r="Y30" s="1">
+        <v>0</v>
+      </c>
       <c r="Z30" s="2"/>
       <c r="AA30" s="1">
         <v>0.0</v>
@@ -9381,9 +9385,7 @@
       <c r="G31" s="1">
         <v>0.0</v>
       </c>
-      <c r="H31" s="2">
-        <v>0.22</v>
-      </c>
+      <c r="H31" s="2"/>
       <c r="I31" s="1"/>
       <c r="J31" s="2"/>
       <c r="K31" s="1"/>
@@ -9412,7 +9414,9 @@
         <v>0</v>
       </c>
       <c r="X31" s="2"/>
-      <c r="Y31" s="1"/>
+      <c r="Y31" s="1">
+        <v>0</v>
+      </c>
       <c r="Z31" s="2"/>
       <c r="AA31" s="1">
         <v>0.0</v>
@@ -9464,9 +9468,7 @@
       <c r="G32" s="1">
         <v>0.0</v>
       </c>
-      <c r="H32" s="2">
-        <v>0.22</v>
-      </c>
+      <c r="H32" s="2"/>
       <c r="I32" s="1"/>
       <c r="J32" s="2"/>
       <c r="K32" s="1"/>
@@ -9495,7 +9497,9 @@
         <v>0</v>
       </c>
       <c r="X32" s="2"/>
-      <c r="Y32" s="1"/>
+      <c r="Y32" s="1">
+        <v>0</v>
+      </c>
       <c r="Z32" s="2"/>
       <c r="AA32" s="1">
         <v>0.0</v>
@@ -9547,9 +9551,7 @@
       <c r="G33" s="1">
         <v>0.0</v>
       </c>
-      <c r="H33" s="2">
-        <v>0.22</v>
-      </c>
+      <c r="H33" s="2"/>
       <c r="I33" s="1"/>
       <c r="J33" s="2"/>
       <c r="K33" s="1"/>
@@ -9578,7 +9580,9 @@
         <v>0</v>
       </c>
       <c r="X33" s="2"/>
-      <c r="Y33" s="1"/>
+      <c r="Y33" s="1">
+        <v>0</v>
+      </c>
       <c r="Z33" s="2"/>
       <c r="AA33" s="1">
         <v>0.0</v>
@@ -9630,9 +9634,7 @@
       <c r="G34" s="1">
         <v>0.0</v>
       </c>
-      <c r="H34" s="2">
-        <v>0.22</v>
-      </c>
+      <c r="H34" s="2"/>
       <c r="I34" s="1"/>
       <c r="J34" s="2"/>
       <c r="K34" s="1"/>
@@ -9661,7 +9663,9 @@
         <v>0</v>
       </c>
       <c r="X34" s="2"/>
-      <c r="Y34" s="1"/>
+      <c r="Y34" s="1">
+        <v>0</v>
+      </c>
       <c r="Z34" s="2"/>
       <c r="AA34" s="1">
         <v>0.0</v>
@@ -9713,9 +9717,7 @@
       <c r="G35" s="1">
         <v>0.0</v>
       </c>
-      <c r="H35" s="2">
-        <v>0.22</v>
-      </c>
+      <c r="H35" s="2"/>
       <c r="I35" s="1"/>
       <c r="J35" s="2"/>
       <c r="K35" s="1"/>
@@ -9744,7 +9746,9 @@
         <v>0</v>
       </c>
       <c r="X35" s="2"/>
-      <c r="Y35" s="1"/>
+      <c r="Y35" s="1">
+        <v>0</v>
+      </c>
       <c r="Z35" s="2"/>
       <c r="AA35" s="1">
         <v>0.0</v>
@@ -9796,9 +9800,7 @@
       <c r="G36" s="1">
         <v>0.0</v>
       </c>
-      <c r="H36" s="2">
-        <v>0.22</v>
-      </c>
+      <c r="H36" s="2"/>
       <c r="I36" s="1"/>
       <c r="J36" s="2"/>
       <c r="K36" s="1"/>
@@ -9827,7 +9829,9 @@
         <v>0</v>
       </c>
       <c r="X36" s="2"/>
-      <c r="Y36" s="1"/>
+      <c r="Y36" s="1">
+        <v>0</v>
+      </c>
       <c r="Z36" s="2"/>
       <c r="AA36" s="1">
         <v>0.0</v>
@@ -9879,9 +9883,7 @@
       <c r="G37" s="1">
         <v>0.0</v>
       </c>
-      <c r="H37" s="2">
-        <v>0.22</v>
-      </c>
+      <c r="H37" s="2"/>
       <c r="I37" s="1"/>
       <c r="J37" s="2"/>
       <c r="K37" s="1"/>
@@ -9910,7 +9912,9 @@
         <v>0</v>
       </c>
       <c r="X37" s="2"/>
-      <c r="Y37" s="1"/>
+      <c r="Y37" s="1">
+        <v>0</v>
+      </c>
       <c r="Z37" s="2"/>
       <c r="AA37" s="1">
         <v>0.0</v>
@@ -10011,8 +10015,12 @@
       <c r="X38" s="2">
         <v>0.01</v>
       </c>
-      <c r="Y38" s="1"/>
-      <c r="Z38" s="2"/>
+      <c r="Y38" s="1">
+        <v>4200.0</v>
+      </c>
+      <c r="Z38" s="2">
+        <v>0.003</v>
+      </c>
       <c r="AA38" s="1">
         <v>3000000.0</v>
       </c>
@@ -10024,10 +10032,10 @@
       </c>
       <c r="AD38" s="2"/>
       <c r="AE38" s="1">
-        <v>-215521.4</v>
+        <v>-219721.4</v>
       </c>
       <c r="AF38" s="1">
-        <v>-215521.4</v>
+        <v>-219721.4</v>
       </c>
       <c r="AG38" s="2">
         <v>0.48640766666667</v>
@@ -10114,8 +10122,12 @@
       <c r="X39" s="9">
         <v>0.01</v>
       </c>
-      <c r="Y39" s="8"/>
-      <c r="Z39" s="9"/>
+      <c r="Y39" s="8">
+        <v>4452.0</v>
+      </c>
+      <c r="Z39" s="9">
+        <v>0.003</v>
+      </c>
       <c r="AA39" s="8">
         <v>3093600.0</v>
       </c>
@@ -10129,10 +10141,10 @@
         <v>0.22</v>
       </c>
       <c r="AE39" s="8">
-        <v>-225466.62</v>
+        <v>-229918.62</v>
       </c>
       <c r="AF39" s="8">
-        <v>-440988.02</v>
+        <v>-449640.02</v>
       </c>
       <c r="AG39" s="9">
         <v>0.45453141025641</v>
@@ -10219,8 +10231,12 @@
       <c r="X40" s="12">
         <v>0.01</v>
       </c>
-      <c r="Y40" s="11"/>
-      <c r="Z40" s="12"/>
+      <c r="Y40" s="11">
+        <v>4779.6</v>
+      </c>
+      <c r="Z40" s="12">
+        <v>0.003</v>
+      </c>
       <c r="AA40" s="11">
         <v>3215280.0</v>
       </c>
@@ -10234,10 +10250,10 @@
         <v>0.22</v>
       </c>
       <c r="AE40" s="11">
-        <v>-219452.5686</v>
+        <v>-224232.1686</v>
       </c>
       <c r="AF40" s="11">
-        <v>-660440.5886</v>
+        <v>-673872.1886</v>
       </c>
       <c r="AG40" s="12">
         <v>0.4182036019536</v>
@@ -10324,8 +10340,12 @@
       <c r="X41" s="2">
         <v>0.01</v>
       </c>
-      <c r="Y41" s="1"/>
-      <c r="Z41" s="2"/>
+      <c r="Y41" s="1">
+        <v>5123.58</v>
+      </c>
+      <c r="Z41" s="2">
+        <v>0.003</v>
+      </c>
       <c r="AA41" s="1">
         <v>3343044.0</v>
       </c>
@@ -10339,10 +10359,10 @@
         <v>0.22</v>
       </c>
       <c r="AE41" s="1">
-        <v>-213566.1056</v>
+        <v>-218689.6856</v>
       </c>
       <c r="AF41" s="1">
-        <v>-874006.6942</v>
+        <v>-892561.8742</v>
       </c>
       <c r="AG41" s="2">
         <v>0.38219111576254</v>
@@ -10429,8 +10449,12 @@
       <c r="X42" s="2">
         <v>0.01</v>
       </c>
-      <c r="Y42" s="1"/>
-      <c r="Z42" s="2"/>
+      <c r="Y42" s="1">
+        <v>5484.759</v>
+      </c>
+      <c r="Z42" s="2">
+        <v>0.003</v>
+      </c>
       <c r="AA42" s="1">
         <v>3477196.2</v>
       </c>
@@ -10444,10 +10468,10 @@
         <v>0.22</v>
       </c>
       <c r="AE42" s="1">
-        <v>-212668.2496</v>
+        <v>-218153.0086</v>
       </c>
       <c r="AF42" s="1">
-        <v>-1086674.9438</v>
+        <v>-1110714.8828</v>
       </c>
       <c r="AG42" s="2">
         <v>0.34731338200726</v>
@@ -10534,8 +10558,12 @@
       <c r="X43" s="2">
         <v>0.01</v>
       </c>
-      <c r="Y43" s="1"/>
-      <c r="Z43" s="2"/>
+      <c r="Y43" s="1">
+        <v>5863.998</v>
+      </c>
+      <c r="Z43" s="2">
+        <v>0.003</v>
+      </c>
       <c r="AA43" s="1">
         <v>3618056.4</v>
       </c>
@@ -10549,10 +10577,10 @@
         <v>0.22</v>
       </c>
       <c r="AE43" s="1">
-        <v>-216088.422</v>
+        <v>-221952.42</v>
       </c>
       <c r="AF43" s="1">
-        <v>-1302763.3658</v>
+        <v>-1332667.3028</v>
       </c>
       <c r="AG43" s="2">
         <v>0.31425542798981</v>
@@ -10639,8 +10667,12 @@
       <c r="X44" s="2">
         <v>0.01</v>
       </c>
-      <c r="Y44" s="1"/>
-      <c r="Z44" s="2"/>
+      <c r="Y44" s="1">
+        <v>6262.1979</v>
+      </c>
+      <c r="Z44" s="2">
+        <v>0.003</v>
+      </c>
       <c r="AA44" s="1">
         <v>3765959.22</v>
       </c>
@@ -10654,10 +10686,10 @@
         <v>0.22</v>
       </c>
       <c r="AE44" s="1">
-        <v>-219631.504</v>
+        <v>-225893.7019</v>
       </c>
       <c r="AF44" s="1">
-        <v>-1522394.8698</v>
+        <v>-1558561.0047</v>
       </c>
       <c r="AG44" s="2">
         <v>0.28292900123782</v>
@@ -10744,8 +10776,12 @@
       <c r="X45" s="2">
         <v>0.01</v>
       </c>
-      <c r="Y45" s="1"/>
-      <c r="Z45" s="2"/>
+      <c r="Y45" s="1">
+        <v>6680.3079</v>
+      </c>
+      <c r="Z45" s="2">
+        <v>0.003</v>
+      </c>
       <c r="AA45" s="1">
         <v>3921257.22</v>
       </c>
@@ -10759,10 +10795,10 @@
         <v>0.22</v>
       </c>
       <c r="AE45" s="1">
-        <v>-223302.0156</v>
+        <v>-229982.3235</v>
       </c>
       <c r="AF45" s="1">
-        <v>-1745696.8854</v>
+        <v>-1788543.3282</v>
       </c>
       <c r="AG45" s="2">
         <v>0.25325016221812</v>
@@ -10849,8 +10885,12 @@
       <c r="X46" s="2">
         <v>0.01</v>
       </c>
-      <c r="Y46" s="1"/>
-      <c r="Z46" s="2"/>
+      <c r="Y46" s="1">
+        <v>7119.3234</v>
+      </c>
+      <c r="Z46" s="2">
+        <v>0.003</v>
+      </c>
       <c r="AA46" s="1">
         <v>4084320.12</v>
       </c>
@@ -10864,10 +10904,10 @@
         <v>0.22</v>
       </c>
       <c r="AE46" s="1">
-        <v>-227106.288</v>
+        <v>-234225.6114</v>
       </c>
       <c r="AF46" s="1">
-        <v>-1972803.1734</v>
+        <v>-2022768.9396</v>
       </c>
       <c r="AG46" s="2">
         <v>0.22513879923119</v>
@@ -10954,8 +10994,12 @@
       <c r="X47" s="2">
         <v>0.01</v>
       </c>
-      <c r="Y47" s="1"/>
-      <c r="Z47" s="2"/>
+      <c r="Y47" s="1">
+        <v>7580.2902</v>
+      </c>
+      <c r="Z47" s="2">
+        <v>0.003</v>
+      </c>
       <c r="AA47" s="1">
         <v>4255536.36</v>
       </c>
@@ -10969,10 +11013,10 @@
         <v>0.22</v>
       </c>
       <c r="AE47" s="1">
-        <v>-231049.3012</v>
+        <v>-238629.5914</v>
       </c>
       <c r="AF47" s="1">
-        <v>-2203852.4746</v>
+        <v>-2261398.531</v>
       </c>
       <c r="AG47" s="2">
         <v>0.19851889357615</v>
@@ -11059,8 +11103,12 @@
       <c r="X48" s="2">
         <v>0.01</v>
       </c>
-      <c r="Y48" s="1"/>
-      <c r="Z48" s="2"/>
+      <c r="Y48" s="1">
+        <v>8064.3045</v>
+      </c>
+      <c r="Z48" s="2">
+        <v>0.003</v>
+      </c>
       <c r="AA48" s="1">
         <v>4435313.1</v>
       </c>
@@ -11074,10 +11122,10 @@
         <v>0.22</v>
       </c>
       <c r="AE48" s="1">
-        <v>-235137.0708</v>
+        <v>-243201.3753</v>
       </c>
       <c r="AF48" s="1">
-        <v>-2438989.5454</v>
+        <v>-2504599.9063</v>
       </c>
       <c r="AG48" s="2">
         <v>0.1733181547247</v>
@@ -11164,8 +11212,12 @@
       <c r="X49" s="2">
         <v>0.01</v>
       </c>
-      <c r="Y49" s="1"/>
-      <c r="Z49" s="2"/>
+      <c r="Y49" s="1">
+        <v>8572.5192</v>
+      </c>
+      <c r="Z49" s="2">
+        <v>0.003</v>
+      </c>
       <c r="AA49" s="1">
         <v>4624078.56</v>
       </c>
@@ -11179,10 +11231,10 @@
         <v>0.22</v>
       </c>
       <c r="AE49" s="1">
-        <v>-239375.0868</v>
+        <v>-247947.606</v>
       </c>
       <c r="AF49" s="1">
-        <v>-2678364.6322</v>
+        <v>-2752547.5123</v>
       </c>
       <c r="AG49" s="2">
         <v>0.14946758774629</v>
@@ -11269,8 +11321,12 @@
       <c r="X50" s="2">
         <v>0.01</v>
       </c>
-      <c r="Y50" s="1"/>
-      <c r="Z50" s="2"/>
+      <c r="Y50" s="1">
+        <v>9106.146</v>
+      </c>
+      <c r="Z50" s="2">
+        <v>0.003</v>
+      </c>
       <c r="AA50" s="1">
         <v>4822282.8</v>
       </c>
@@ -11284,10 +11340,10 @@
         <v>0.22</v>
       </c>
       <c r="AE50" s="1">
-        <v>-243770.7104</v>
+        <v>-252876.8564</v>
       </c>
       <c r="AF50" s="1">
-        <v>-2922135.3426</v>
+        <v>-3005424.3687</v>
       </c>
       <c r="AG50" s="2">
         <v>0.12690105054851</v>
@@ -11374,8 +11430,12 @@
       <c r="X51" s="2">
         <v>0.01</v>
       </c>
-      <c r="Y51" s="1"/>
-      <c r="Z51" s="2"/>
+      <c r="Y51" s="1">
+        <v>9666.4533</v>
+      </c>
+      <c r="Z51" s="2">
+        <v>0.003</v>
+      </c>
       <c r="AA51" s="1">
         <v>5030396.94</v>
       </c>
@@ -11389,10 +11449,10 @@
         <v>0.22</v>
       </c>
       <c r="AE51" s="1">
-        <v>-248330.7772</v>
+        <v>-257997.2305</v>
       </c>
       <c r="AF51" s="1">
-        <v>-3170466.1198</v>
+        <v>-3263421.5992</v>
       </c>
       <c r="AG51" s="2">
         <v>0.10555636166082</v>
@@ -11479,8 +11539,12 @@
       <c r="X52" s="2">
         <v>0.01</v>
       </c>
-      <c r="Y52" s="1"/>
-      <c r="Z52" s="2"/>
+      <c r="Y52" s="1">
+        <v>10254.7767</v>
+      </c>
+      <c r="Z52" s="2">
+        <v>0.003</v>
+      </c>
       <c r="AA52" s="1">
         <v>5248917.06</v>
       </c>
@@ -11494,10 +11558,10 @@
         <v>0.22</v>
       </c>
       <c r="AE52" s="1">
-        <v>-253061.6472</v>
+        <v>-263316.4239</v>
       </c>
       <c r="AF52" s="1">
-        <v>-3423527.767</v>
+        <v>-3526738.0231</v>
       </c>
       <c r="AG52" s="2">
         <v>0.085373724318304</v>
@@ -11584,8 +11648,12 @@
       <c r="X53" s="14">
         <v>0.01</v>
       </c>
-      <c r="Y53" s="13"/>
-      <c r="Z53" s="14"/>
+      <c r="Y53" s="13">
+        <v>10872.5148</v>
+      </c>
+      <c r="Z53" s="14">
+        <v>0.003</v>
+      </c>
       <c r="AA53" s="13">
         <v>5478362.64</v>
       </c>
@@ -11599,10 +11667,10 @@
         <v>0.22</v>
       </c>
       <c r="AE53" s="13">
-        <v>-257971.5716</v>
+        <v>-268844.0864</v>
       </c>
       <c r="AF53" s="13">
-        <v>-3681499.3386</v>
+        <v>-3795582.1095</v>
       </c>
       <c r="AG53" s="14">
         <v>0.066296628931192</v>
@@ -11689,8 +11757,12 @@
       <c r="X54" s="2">
         <v>0.01</v>
       </c>
-      <c r="Y54" s="1"/>
-      <c r="Z54" s="2"/>
+      <c r="Y54" s="1">
+        <v>11521.1397</v>
+      </c>
+      <c r="Z54" s="2">
+        <v>0.003</v>
+      </c>
       <c r="AA54" s="1">
         <v>5719280.46</v>
       </c>
@@ -11704,10 +11776,10 @@
         <v>0.22</v>
       </c>
       <c r="AE54" s="1">
-        <v>-263067.5604</v>
+        <v>-274588.7001</v>
       </c>
       <c r="AF54" s="1">
-        <v>-3944566.899</v>
+        <v>-4070170.8096</v>
       </c>
       <c r="AG54" s="2">
         <v>0.048270828615024</v>
@@ -11794,8 +11866,12 @@
       <c r="X55" s="2">
         <v>0.01</v>
       </c>
-      <c r="Y55" s="1"/>
-      <c r="Z55" s="2"/>
+      <c r="Y55" s="1">
+        <v>12202.197</v>
+      </c>
+      <c r="Z55" s="2">
+        <v>0.003</v>
+      </c>
       <c r="AA55" s="1">
         <v>5972244.6</v>
       </c>
@@ -11809,10 +11885,10 @@
         <v>0.22</v>
       </c>
       <c r="AE55" s="1">
-        <v>-268358.5648</v>
+        <v>-280560.7618</v>
       </c>
       <c r="AF55" s="1">
-        <v>-4212925.4638</v>
+        <v>-4350731.5714</v>
       </c>
       <c r="AG55" s="2">
         <v>0.031245108706026</v>
@@ -11899,8 +11975,12 @@
       <c r="X56" s="2">
         <v>0.01</v>
       </c>
-      <c r="Y56" s="1"/>
-      <c r="Z56" s="2"/>
+      <c r="Y56" s="1">
+        <v>12917.3079</v>
+      </c>
+      <c r="Z56" s="2">
+        <v>0.003</v>
+      </c>
       <c r="AA56" s="1">
         <v>6237857.22</v>
       </c>
@@ -11914,10 +11994,10 @@
         <v>0.22</v>
       </c>
       <c r="AE56" s="1">
-        <v>-273852.3048</v>
+        <v>-286769.6127</v>
       </c>
       <c r="AF56" s="1">
-        <v>-4486777.7686</v>
+        <v>-4637501.1841</v>
       </c>
       <c r="AG56" s="2">
         <v>0.015170395487463</v>
@@ -12004,8 +12084,12 @@
       <c r="X57" s="14">
         <v>0.01</v>
       </c>
-      <c r="Y57" s="13"/>
-      <c r="Z57" s="14"/>
+      <c r="Y57" s="13">
+        <v>13668.1734</v>
+      </c>
+      <c r="Z57" s="14">
+        <v>0.003</v>
+      </c>
       <c r="AA57" s="13">
         <v>6516750.12</v>
       </c>
@@ -12019,10 +12103,10 @@
         <v>0.22</v>
       </c>
       <c r="AE57" s="13">
-        <v>-279558.4716</v>
+        <v>-293226.645</v>
       </c>
       <c r="AF57" s="13">
-        <v>-4766336.2402</v>
+        <v>-4930727.8291</v>
       </c>
       <c r="AG57" s="14"/>
       <c r="AH57" s="13">
@@ -12097,8 +12181,12 @@
       <c r="X58" s="2">
         <v>0.01</v>
       </c>
-      <c r="Y58" s="1"/>
-      <c r="Z58" s="2"/>
+      <c r="Y58" s="1">
+        <v>14456.5827</v>
+      </c>
+      <c r="Z58" s="2">
+        <v>0.003</v>
+      </c>
       <c r="AA58" s="1">
         <v>6809587.86</v>
       </c>
@@ -12112,10 +12200,10 @@
         <v>0.22</v>
       </c>
       <c r="AE58" s="1">
-        <v>-172661.5852</v>
+        <v>-187118.1679</v>
       </c>
       <c r="AF58" s="1">
-        <v>-4938997.8254</v>
+        <v>-5117845.997</v>
       </c>
       <c r="AG58" s="2"/>
       <c r="AH58" s="1">
@@ -12190,8 +12278,12 @@
       <c r="X59" s="2">
         <v>0.01</v>
       </c>
-      <c r="Y59" s="1"/>
-      <c r="Z59" s="2"/>
+      <c r="Y59" s="1">
+        <v>15284.4111</v>
+      </c>
+      <c r="Z59" s="2">
+        <v>0.003</v>
+      </c>
       <c r="AA59" s="1">
         <v>7117066.98</v>
       </c>
@@ -12205,10 +12297,10 @@
         <v>0.22</v>
       </c>
       <c r="AE59" s="1">
-        <v>-178820.1668</v>
+        <v>-194104.5779</v>
       </c>
       <c r="AF59" s="1">
-        <v>-5117817.9922</v>
+        <v>-5311950.5749</v>
       </c>
       <c r="AG59" s="2"/>
       <c r="AH59" s="1">
@@ -12283,8 +12375,12 @@
       <c r="X60" s="2">
         <v>0.01</v>
       </c>
-      <c r="Y60" s="1"/>
-      <c r="Z60" s="2"/>
+      <c r="Y60" s="1">
+        <v>16153.6326</v>
+      </c>
+      <c r="Z60" s="2">
+        <v>0.003</v>
+      </c>
       <c r="AA60" s="1">
         <v>7439920.68</v>
       </c>
@@ -12298,10 +12394,10 @@
         <v>0.22</v>
       </c>
       <c r="AE60" s="1">
-        <v>-185220.412</v>
+        <v>-201374.0446</v>
       </c>
       <c r="AF60" s="1">
-        <v>-5303038.4042</v>
+        <v>-5513324.6195</v>
       </c>
       <c r="AG60" s="2"/>
       <c r="AH60" s="1">
@@ -12376,8 +12472,12 @@
       <c r="X61" s="2">
         <v>0.01</v>
       </c>
-      <c r="Y61" s="1"/>
-      <c r="Z61" s="2"/>
+      <c r="Y61" s="1">
+        <v>17066.3136</v>
+      </c>
+      <c r="Z61" s="2">
+        <v>0.003</v>
+      </c>
       <c r="AA61" s="1">
         <v>7778916.48</v>
       </c>
@@ -12391,10 +12491,10 @@
         <v>0.22</v>
       </c>
       <c r="AE61" s="1">
-        <v>-191872.1608</v>
+        <v>-208938.4744</v>
       </c>
       <c r="AF61" s="1">
-        <v>-5494910.565</v>
+        <v>-5722263.0939</v>
       </c>
       <c r="AG61" s="2"/>
       <c r="AH61" s="1">
@@ -12469,8 +12569,12 @@
       <c r="X62" s="2">
         <v>0.01</v>
       </c>
-      <c r="Y62" s="1"/>
-      <c r="Z62" s="2"/>
+      <c r="Y62" s="1">
+        <v>18024.6297</v>
+      </c>
+      <c r="Z62" s="2">
+        <v>0.003</v>
+      </c>
       <c r="AA62" s="1">
         <v>8134862.46</v>
       </c>
@@ -12484,10 +12588,10 @@
         <v>0.22</v>
       </c>
       <c r="AE62" s="1">
-        <v>-198787.3644</v>
+        <v>-216811.9941</v>
       </c>
       <c r="AF62" s="1">
-        <v>-5693697.9294</v>
+        <v>-5939075.088</v>
       </c>
       <c r="AG62" s="2"/>
       <c r="AH62" s="1">
@@ -12562,8 +12666,12 @@
       <c r="X63" s="2">
         <v>0.01</v>
       </c>
-      <c r="Y63" s="1"/>
-      <c r="Z63" s="2"/>
+      <c r="Y63" s="1">
+        <v>19030.8615</v>
+      </c>
+      <c r="Z63" s="2">
+        <v>0.003</v>
+      </c>
       <c r="AA63" s="1">
         <v>8508605.7</v>
       </c>
@@ -12577,10 +12685,10 @@
         <v>0.22</v>
       </c>
       <c r="AE63" s="1">
-        <v>-205977.6784</v>
+        <v>-225008.5399</v>
       </c>
       <c r="AF63" s="1">
-        <v>-5899675.6078</v>
+        <v>-6164083.6279</v>
       </c>
       <c r="AG63" s="2"/>
       <c r="AH63" s="1">
@@ -12655,8 +12763,12 @@
       <c r="X64" s="2">
         <v>0.01</v>
       </c>
-      <c r="Y64" s="1"/>
-      <c r="Z64" s="2"/>
+      <c r="Y64" s="1">
+        <v>20087.4051</v>
+      </c>
+      <c r="Z64" s="2">
+        <v>0.003</v>
+      </c>
       <c r="AA64" s="1">
         <v>8901036.18</v>
       </c>
@@ -12670,10 +12782,10 @@
         <v>0.22</v>
       </c>
       <c r="AE64" s="1">
-        <v>-213456.104</v>
+        <v>-233543.5091</v>
       </c>
       <c r="AF64" s="1">
-        <v>-6113131.7118</v>
+        <v>-6397627.137</v>
       </c>
       <c r="AG64" s="2"/>
       <c r="AH64" s="1">
@@ -12748,8 +12860,12 @@
       <c r="X65" s="2">
         <v>0.01</v>
       </c>
-      <c r="Y65" s="1"/>
-      <c r="Z65" s="2"/>
+      <c r="Y65" s="1">
+        <v>21196.7763</v>
+      </c>
+      <c r="Z65" s="2">
+        <v>0.003</v>
+      </c>
       <c r="AA65" s="1">
         <v>9313088.34</v>
       </c>
@@ -12763,10 +12879,10 @@
         <v>0.22</v>
       </c>
       <c r="AE65" s="1">
-        <v>-221234.6212</v>
+        <v>-242431.3975</v>
       </c>
       <c r="AF65" s="1">
-        <v>-6334366.333</v>
+        <v>-6640058.5345</v>
       </c>
       <c r="AG65" s="2"/>
       <c r="AH65" s="1">
@@ -12841,8 +12957,12 @@
       <c r="X66" s="2">
         <v>0.01</v>
       </c>
-      <c r="Y66" s="1"/>
-      <c r="Z66" s="2"/>
+      <c r="Y66" s="1">
+        <v>22361.6148</v>
+      </c>
+      <c r="Z66" s="2">
+        <v>0.003</v>
+      </c>
       <c r="AA66" s="1">
         <v>9745742.64</v>
       </c>
@@ -12856,10 +12976,10 @@
         <v>0.22</v>
       </c>
       <c r="AE66" s="1">
-        <v>-229327.3912</v>
+        <v>-251689.006</v>
       </c>
       <c r="AF66" s="1">
-        <v>-6563693.7242</v>
+        <v>-6891747.5405</v>
       </c>
       <c r="AG66" s="2"/>
       <c r="AH66" s="1">
@@ -12934,8 +13054,12 @@
       <c r="X67" s="2">
         <v>0.01</v>
       </c>
-      <c r="Y67" s="1"/>
-      <c r="Z67" s="2"/>
+      <c r="Y67" s="1">
+        <v>23584.6947</v>
+      </c>
+      <c r="Z67" s="2">
+        <v>0.003</v>
+      </c>
       <c r="AA67" s="1">
         <v>10200029.46</v>
       </c>
@@ -12949,10 +13073,10 @@
         <v>0.22</v>
       </c>
       <c r="AE67" s="1">
-        <v>-237748.4196</v>
+        <v>-261333.1143</v>
       </c>
       <c r="AF67" s="1">
-        <v>-6801442.1438</v>
+        <v>-7153080.6548</v>
       </c>
       <c r="AG67" s="2"/>
       <c r="AH67" s="1">
@@ -13027,8 +13151,12 @@
       <c r="X68" s="2">
         <v>0.01</v>
       </c>
-      <c r="Y68" s="1"/>
-      <c r="Z68" s="2"/>
+      <c r="Y68" s="1">
+        <v>24868.9287</v>
+      </c>
+      <c r="Z68" s="2">
+        <v>0.003</v>
+      </c>
       <c r="AA68" s="1">
         <v>10677030.66</v>
       </c>
@@ -13042,10 +13170,10 @@
         <v>0.22</v>
       </c>
       <c r="AE68" s="1">
-        <v>-246512.372</v>
+        <v>-271381.3007</v>
       </c>
       <c r="AF68" s="1">
-        <v>-7047954.5158</v>
+        <v>-7424461.9555</v>
       </c>
       <c r="AG68" s="2"/>
       <c r="AH68" s="1">
@@ -13120,8 +13248,12 @@
       <c r="X69" s="2">
         <v>0.01</v>
       </c>
-      <c r="Y69" s="1"/>
-      <c r="Z69" s="2"/>
+      <c r="Y69" s="1">
+        <v>26217.3744</v>
+      </c>
+      <c r="Z69" s="2">
+        <v>0.003</v>
+      </c>
       <c r="AA69" s="1">
         <v>11177881.92</v>
       </c>
@@ -13135,10 +13267,10 @@
         <v>0.22</v>
       </c>
       <c r="AE69" s="1">
-        <v>-255635.3996</v>
+        <v>-281852.774</v>
       </c>
       <c r="AF69" s="1">
-        <v>-7303589.9154</v>
+        <v>-7706314.7295</v>
       </c>
       <c r="AG69" s="2"/>
       <c r="AH69" s="1">
@@ -13213,8 +13345,12 @@
       <c r="X70" s="2">
         <v>0.01</v>
       </c>
-      <c r="Y70" s="1"/>
-      <c r="Z70" s="2"/>
+      <c r="Y70" s="1">
+        <v>27633.2427</v>
+      </c>
+      <c r="Z70" s="2">
+        <v>0.003</v>
+      </c>
       <c r="AA70" s="1">
         <v>11703775.86</v>
       </c>
@@ -13228,10 +13364,10 @@
         <v>0.22</v>
       </c>
       <c r="AE70" s="1">
-        <v>-265133.588</v>
+        <v>-292766.8307</v>
       </c>
       <c r="AF70" s="1">
-        <v>-7568723.5034</v>
+        <v>-7999081.5602</v>
       </c>
       <c r="AG70" s="2"/>
       <c r="AH70" s="1">
@@ -13306,8 +13442,12 @@
       <c r="X71" s="2">
         <v>0.01</v>
       </c>
-      <c r="Y71" s="1"/>
-      <c r="Z71" s="2"/>
+      <c r="Y71" s="1">
+        <v>29119.9041</v>
+      </c>
+      <c r="Z71" s="2">
+        <v>0.003</v>
+      </c>
       <c r="AA71" s="1">
         <v>12255964.38</v>
       </c>
@@ -13321,10 +13461,10 @@
         <v>0.22</v>
       </c>
       <c r="AE71" s="1">
-        <v>-275023.7828</v>
+        <v>-304143.6869</v>
       </c>
       <c r="AF71" s="1">
-        <v>-7843747.2862</v>
+        <v>-8303225.2471</v>
       </c>
       <c r="AG71" s="2"/>
       <c r="AH71" s="1">
@@ -13399,8 +13539,12 @@
       <c r="X72" s="16">
         <v>0.01</v>
       </c>
-      <c r="Y72" s="5"/>
-      <c r="Z72" s="16"/>
+      <c r="Y72" s="5">
+        <v>30680.8992</v>
+      </c>
+      <c r="Z72" s="16">
+        <v>0.003</v>
+      </c>
       <c r="AA72" s="5">
         <v>12835762.56</v>
       </c>
@@ -13414,10 +13558,10 @@
         <v>0.22</v>
       </c>
       <c r="AE72" s="5">
-        <v>-285324.4352</v>
+        <v>-316005.3344</v>
       </c>
       <c r="AF72" s="5">
-        <v>-8129071.7214</v>
+        <v>-8619230.5815</v>
       </c>
       <c r="AG72" s="16"/>
       <c r="AH72" s="5">

</xml_diff>